<commit_message>
streamline auth, casual attendance
</commit_message>
<xml_diff>
--- a/DBMS/DPL_Model.xlsx
+++ b/DBMS/DPL_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\DPL_web\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0415D4A-1DB0-480E-B169-B49184BC59BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F3EA85-B85F-4AFE-9698-36786AD010D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Table Name</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Doj</t>
   </si>
   <si>
-    <t>Home page without sign-in</t>
-  </si>
-  <si>
     <t>HoD</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>View shift schedule of all employees for today only[a.k.a. Homepage]</t>
-  </si>
-  <si>
     <t>G-shift I/c</t>
   </si>
   <si>
@@ -161,18 +155,6 @@
     <t>Area Head</t>
   </si>
   <si>
-    <t xml:space="preserve"> + View deptt wise employee and cauals list, View deptt wise plant dashboard, view deptt profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Manage self profile, edit/create self shift schedule, attendance of reporting casuals</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + edit/create shift schedule of all reporting employees, View casual attendance fed by lower level</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + edit/create shift schedule of all employees reporting to HoD</t>
-  </si>
-  <si>
     <t>Contractors</t>
   </si>
   <si>
@@ -221,12 +203,6 @@
     <t>Generate custome reports</t>
   </si>
   <si>
-    <t xml:space="preserve"> + Edit/create contract details</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> + Edit/create employee profiles, Edit deptt profile, other powers</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
@@ -264,6 +240,39 @@
   </si>
   <si>
     <t>System Admin</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>No previlage Employees</t>
+  </si>
+  <si>
+    <t>{home}</t>
+  </si>
+  <si>
+    <t>{home} =&gt; all available shift I/Cs</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard}</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}}</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan}}</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan, password_reset, create user, delete user, view casual attendance}}</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan, password_reset, create user, delete user, view casual attendance, create contract, edit contract, add caual, reamove casual}}</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{view casual attendance, create contract, edit contract, add caual, reamove casual}}</t>
+  </si>
+  <si>
+    <t>DPL Admin</t>
   </si>
 </sst>
 </file>
@@ -776,16 +785,16 @@
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.35">
@@ -802,13 +811,13 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
         <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
         <v>17</v>
@@ -822,19 +831,19 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -842,22 +851,22 @@
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -868,16 +877,16 @@
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -885,13 +894,13 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -899,10 +908,10 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -910,7 +919,7 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -918,7 +927,7 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -934,7 +943,7 @@
         <v>4</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -942,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -952,7 +961,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -978,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -998,10 +1007,10 @@
         <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>15</v>
@@ -1012,104 +1021,126 @@
         <v>10</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>700</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
-        <v>90</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>43</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>600</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>500</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1124,30 +1155,30 @@
       <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14"/>
-      <c r="B14"/>
-      <c r="C14"/>
-      <c r="D14"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>900</v>
       </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17"/>
@@ -1155,39 +1186,39 @@
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="21" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
-        <v>100</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>62</v>
-      </c>
+    <row r="18" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
     </row>
     <row r="22" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
+        <v>100</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11">
         <v>200</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="10"/>
+      <c r="D23" s="10" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
@@ -1207,6 +1238,12 @@
       <c r="C26" s="11"/>
       <c r="D26" s="10"/>
     </row>
+    <row r="27" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implement RBAC in express app
</commit_message>
<xml_diff>
--- a/DBMS/DPL_Model.xlsx
+++ b/DBMS/DPL_Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\DPL_web\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F3EA85-B85F-4AFE-9698-36786AD010D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8817FEFE-EE22-4364-8123-3A50C87409CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="91">
   <si>
     <t>Table Name</t>
   </si>
@@ -266,20 +266,50 @@
     <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan, password_reset, create user, delete user, view casual attendance}}</t>
   </si>
   <si>
-    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan, password_reset, create user, delete user, view casual attendance, create contract, edit contract, add caual, reamove casual}}</t>
-  </si>
-  <si>
     <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{view casual attendance, create contract, edit contract, add caual, reamove casual}}</t>
   </si>
   <si>
     <t>DPL Admin</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>dept</t>
+  </si>
+  <si>
+    <t>dashboard</t>
+  </si>
+  <si>
+    <t>profile</t>
+  </si>
+  <si>
+    <t>attendance</t>
+  </si>
+  <si>
+    <t>[Employess, Casuals]</t>
+  </si>
+  <si>
+    <t>[details, shift schedule]</t>
+  </si>
+  <si>
+    <t>[shift plan, password reset, create user, delete user, view casual attendance]</t>
+  </si>
+  <si>
+    <t>[casual]</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>{home, dept:{employees, casuals}, dashboard, profile:{details, shift_schedule}, attendance: {casual}, admin:{shift_plan, password_reset, create user, delete user, view casual attendance, , create contract, edit contract, add caual, reamove casual}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,8 +354,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -347,8 +385,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -371,14 +414,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -412,9 +471,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -987,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -998,11 +1065,17 @@
     <col min="1" max="1" width="8.6640625" style="2"/>
     <col min="2" max="2" width="23.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="27" style="2" customWidth="1"/>
-    <col min="4" max="4" width="121.44140625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="8.6640625" style="2"/>
+    <col min="4" max="4" width="100.21875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>13</v>
       </c>
@@ -1015,8 +1088,26 @@
       <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12">
         <v>10</v>
       </c>
@@ -1029,22 +1120,40 @@
       <c r="D2" s="12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="13">
         <v>700</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="17.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>1</v>
       </c>
@@ -1057,8 +1166,26 @@
       <c r="D4" s="7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>600</v>
       </c>
@@ -1066,13 +1193,31 @@
         <v>54</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>90</v>
       </c>
@@ -1086,7 +1231,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>100</v>
       </c>
@@ -1099,8 +1244,23 @@
       <c r="D8" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>200</v>
       </c>
@@ -1113,8 +1273,23 @@
       <c r="D9" s="9" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>400</v>
       </c>
@@ -1128,7 +1303,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>500</v>
       </c>
@@ -1139,34 +1314,34 @@
         <v>25</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
     </row>
-    <row r="16" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>900</v>
       </c>
@@ -1217,7 +1392,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>